<commit_message>
updated results with new hyperparameter
</commit_message>
<xml_diff>
--- a/tables/mnist_basic_5.xlsx
+++ b/tables/mnist_basic_5.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,10 +612,10 @@
         <v>87.59999999999999</v>
       </c>
       <c r="I4" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J4" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K4" t="n">
         <v>4.8</v>
@@ -654,10 +654,10 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J5" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K5" t="n">
         <v>4.8</v>
@@ -696,10 +696,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J6" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K6" t="n">
         <v>4.8</v>
@@ -738,10 +738,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J7" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K7" t="n">
         <v>4.8</v>
@@ -780,10 +780,10 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J8" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K8" t="n">
         <v>4.8</v>
@@ -826,10 +826,10 @@
         <v>48.4</v>
       </c>
       <c r="I9" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J9" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K9" t="n">
         <v>4.8</v>
@@ -868,10 +868,10 @@
         <v>21.7</v>
       </c>
       <c r="I10" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J10" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K10" t="n">
         <v>4.8</v>
@@ -910,10 +910,10 @@
         <v>2.9</v>
       </c>
       <c r="I11" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J11" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K11" t="n">
         <v>4.8</v>
@@ -952,10 +952,10 @@
         <v>0.5</v>
       </c>
       <c r="I12" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J12" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K12" t="n">
         <v>4.8</v>
@@ -976,9 +976,7 @@
           <t>boundary</t>
         </is>
       </c>
-      <c r="B13" s="1" t="n">
-        <v>0.3</v>
-      </c>
+      <c r="B13" s="1" t="inlineStr"/>
       <c r="C13" t="n">
         <v>100</v>
       </c>
@@ -1044,10 +1042,10 @@
         <v>82.69999999999997</v>
       </c>
       <c r="I14" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J14" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K14" t="n">
         <v>4.8</v>
@@ -1086,10 +1084,10 @@
         <v>13.2</v>
       </c>
       <c r="I15" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J15" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K15" t="n">
         <v>4.8</v>
@@ -1128,10 +1126,10 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J16" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K16" t="n">
         <v>4.8</v>
@@ -1174,10 +1172,10 @@
         <v>3.8</v>
       </c>
       <c r="I17" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J17" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K17" t="n">
         <v>4.8</v>
@@ -1220,10 +1218,10 @@
         <v>85.3</v>
       </c>
       <c r="I18" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J18" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K18" t="n">
         <v>4.8</v>
@@ -1262,10 +1260,10 @@
         <v>8.200000000000001</v>
       </c>
       <c r="I19" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J19" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K19" t="n">
         <v>4.8</v>
@@ -1304,10 +1302,10 @@
         <v>1.1</v>
       </c>
       <c r="I20" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J20" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K20" t="n">
         <v>4.8</v>
@@ -1346,10 +1344,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="I21" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J21" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K21" t="n">
         <v>4.8</v>
@@ -1388,10 +1386,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="I22" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J22" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K22" t="n">
         <v>4.8</v>
@@ -1413,37 +1411,37 @@
         </is>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>99.7</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>99.7</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="E23" t="n">
-        <v>100</v>
+        <v>99.09999999999999</v>
       </c>
       <c r="F23" t="n">
-        <v>99.59999999999999</v>
+        <v>96.8</v>
       </c>
       <c r="G23" t="n">
-        <v>99.3</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="H23" t="n">
-        <v>97.3</v>
+        <v>92.5</v>
       </c>
       <c r="I23" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J23" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K23" t="n">
         <v>4.8</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M23" t="n">
         <v>0.2</v>
@@ -1453,33 +1451,37 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n"/>
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>watermark</t>
+        </is>
+      </c>
       <c r="B24" s="1" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C24" t="n">
-        <v>99.7</v>
+        <v>98.8</v>
       </c>
       <c r="D24" t="n">
-        <v>99.7</v>
+        <v>98.8</v>
       </c>
       <c r="E24" t="n">
         <v>100</v>
       </c>
       <c r="F24" t="n">
+        <v>98.40000000000001</v>
+      </c>
+      <c r="G24" t="n">
         <v>99</v>
       </c>
-      <c r="G24" t="n">
-        <v>99.59999999999999</v>
-      </c>
       <c r="H24" t="n">
-        <v>96.90000000000001</v>
+        <v>97.40000000000001</v>
       </c>
       <c r="I24" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J24" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K24" t="n">
         <v>4.8</v>
@@ -1497,37 +1499,37 @@
     <row r="25">
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C25" t="n">
-        <v>99.8</v>
+        <v>95</v>
       </c>
       <c r="D25" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E25" t="n">
-        <v>99.09999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="F25" t="n">
-        <v>96.8</v>
+        <v>93.7</v>
       </c>
       <c r="G25" t="n">
-        <v>98.40000000000001</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="H25" t="n">
-        <v>92.5</v>
+        <v>91.7</v>
       </c>
       <c r="I25" t="n">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="J25" t="n">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="K25" t="n">
         <v>4.8</v>
       </c>
       <c r="L25" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
         <v>0.2</v>
@@ -1536,104 +1538,15 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>watermark</t>
-        </is>
-      </c>
-      <c r="B26" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="C26" t="n">
-        <v>98.90000000000001</v>
-      </c>
-      <c r="D26" t="n">
-        <v>99.09999999999999</v>
-      </c>
-      <c r="E26" t="n">
-        <v>100</v>
-      </c>
-      <c r="F26" t="n">
-        <v>98.40000000000001</v>
-      </c>
-      <c r="G26" t="n">
-        <v>99</v>
-      </c>
-      <c r="H26" t="n">
-        <v>97.40000000000001</v>
-      </c>
-      <c r="I26" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="J26" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="K26" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="N26" t="n">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C27" t="n">
-        <v>95.5</v>
-      </c>
-      <c r="D27" t="n">
-        <v>96</v>
-      </c>
-      <c r="E27" t="n">
-        <v>98.40000000000001</v>
-      </c>
-      <c r="F27" t="n">
-        <v>93.7</v>
-      </c>
-      <c r="G27" t="n">
-        <v>93.59999999999999</v>
-      </c>
-      <c r="H27" t="n">
-        <v>91.7</v>
-      </c>
-      <c r="I27" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="J27" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="K27" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="N27" t="n">
-        <v>1.5</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A24:A25"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>